<commit_message>
Update: Login to AuthenticationTest
</commit_message>
<xml_diff>
--- a/src/test/java/com/nurfatinportfolio/TestData/products.xlsx
+++ b/src/test/java/com/nurfatinportfolio/TestData/products.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\huawe\eclipse-workspace\SauceDemo\src\test\java\com\nurfatinportfolio\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4827B898-ED24-49DB-9D45-E45E21F6005E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3FC1F8D-61F2-49A4-97DF-00F8152B9380}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="14">
   <si>
     <t>Sauce Labs Bolt T-Shirt</t>
   </si>
@@ -58,6 +58,15 @@
   </si>
   <si>
     <t>RemoveProduct2</t>
+  </si>
+  <si>
+    <t>ProductQty1</t>
+  </si>
+  <si>
+    <t>ProductQty2</t>
+  </si>
+  <si>
+    <t>ProductQty3</t>
   </si>
 </sst>
 </file>
@@ -375,92 +384,137 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="F3" sqref="F3:F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="7" width="25.77734375" customWidth="1"/>
+    <col min="1" max="1" width="25.77734375" customWidth="1"/>
+    <col min="2" max="2" width="14.77734375" customWidth="1"/>
+    <col min="3" max="3" width="25.77734375" customWidth="1"/>
+    <col min="4" max="4" width="14.77734375" customWidth="1"/>
+    <col min="5" max="5" width="25.77734375" customWidth="1"/>
+    <col min="6" max="6" width="14.77734375" customWidth="1"/>
+    <col min="7" max="10" width="25.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>6</v>
       </c>
       <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
         <v>7</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" t="s">
         <v>8</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" t="s">
         <v>9</v>
       </c>
-      <c r="E1" t="s">
+      <c r="H1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2">
         <v>1</v>
       </c>
       <c r="C2" t="s">
         <v>1</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2" t="s">
         <v>2</v>
       </c>
-      <c r="E2" t="s">
+      <c r="H2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B3" t="s">
-        <v>2</v>
-      </c>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C3" t="s">
         <v>2</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3" t="s">
         <v>0</v>
       </c>
-      <c r="E3" t="s">
+      <c r="H3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B4" t="s">
-        <v>0</v>
-      </c>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C4" t="s">
         <v>0</v>
       </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
       <c r="E4" t="s">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="H4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C5" t="s">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E5" t="s">
         <v>4</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="H5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C6" t="s">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E6" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C7" t="s">
+      <c r="F6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E7" t="s">
         <v>5</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>